<commit_message>
Resolved Issue #8 Duplicate lines in BOM
</commit_message>
<xml_diff>
--- a/Beaglebone CAN Cape BOM.xlsx
+++ b/Beaglebone CAN Cape BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim\Documents\BBB Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim\Documents\BeagleBone-CAN-Backpack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="150">
   <si>
     <t>Qty</t>
   </si>
@@ -144,9 +144,6 @@
     <t>C1608X7R1E104K080AA</t>
   </si>
   <si>
-    <t>C50</t>
-  </si>
-  <si>
     <t>TDK</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Capacitor, Ceramic, .1uF 25V 10% 0603 X7R</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>GRM32RR71H105KA01L</t>
   </si>
   <si>
@@ -258,9 +252,6 @@
     <t>ERJ-3EKF5601V</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>64R5354</t>
   </si>
   <si>
@@ -459,28 +450,25 @@
     <t xml:space="preserve">Vendor Part </t>
   </si>
   <si>
-    <t>C7, C8, C9, C10</t>
-  </si>
-  <si>
     <t>R5, R6, R7</t>
   </si>
   <si>
-    <t>R8, R9</t>
-  </si>
-  <si>
     <t>C3, C4</t>
   </si>
   <si>
     <t>R38, R43</t>
   </si>
   <si>
-    <t>R10, R11</t>
-  </si>
-  <si>
     <t>D6, D7</t>
   </si>
   <si>
     <t>Designator</t>
+  </si>
+  <si>
+    <t>C50, C2, C7, C8, C9, C10</t>
+  </si>
+  <si>
+    <t>R3, R8, R9</t>
   </si>
 </sst>
 </file>
@@ -1287,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J11:J12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,22 +1302,22 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" t="s">
         <v>142</v>
-      </c>
-      <c r="E1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" t="s">
-        <v>145</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1508,16 +1496,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -1526,13 +1514,13 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1540,25 +1528,25 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H9">
-        <v>1.0999999999999999E-2</v>
+        <v>0.248</v>
       </c>
       <c r="I9" t="s">
         <v>45</v>
@@ -1566,31 +1554,31 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10">
-        <v>1.0999999999999999E-2</v>
+        <v>52</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
       </c>
       <c r="I10" t="s">
-        <v>146</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1598,28 +1586,28 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="H11">
-        <v>0.248</v>
+        <v>1.2E-2</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1627,28 +1615,28 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
         <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="H12">
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1656,28 +1644,28 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H13">
-        <v>1.2E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1685,115 +1673,115 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F14" t="s">
         <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H14">
-        <v>1.7000000000000001E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15">
-        <v>3.6999999999999998E-2</v>
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
         <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="H16">
-        <v>6.0000000000000001E-3</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="H17">
+        <v>0.35499999999999998</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1801,115 +1789,115 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s">
         <v>32</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H18">
-        <v>9.6000000000000002E-2</v>
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="H19">
-        <v>9.6000000000000002E-2</v>
+        <v>0.47</v>
       </c>
       <c r="I19" t="s">
-        <v>148</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
         <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="H20">
-        <v>0.35499999999999998</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" t="s">
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="H21">
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="I21" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1917,86 +1905,86 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="H22">
-        <v>0.47</v>
+        <v>1.06</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="H23">
-        <v>9.0999999999999998E-2</v>
+        <v>0.872</v>
       </c>
       <c r="I23" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>101</v>
-      </c>
-      <c r="H24">
-        <v>9.6000000000000002E-2</v>
+        <v>113</v>
+      </c>
+      <c r="H24" t="s">
+        <v>115</v>
       </c>
       <c r="I24" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2004,28 +1992,28 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25">
-        <v>1.06</v>
+        <v>119</v>
+      </c>
+      <c r="H25" t="s">
+        <v>121</v>
       </c>
       <c r="I25" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2033,28 +2021,28 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="H26">
-        <v>0.872</v>
+        <v>2.72</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2062,28 +2050,28 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" t="s">
-        <v>118</v>
+        <v>129</v>
+      </c>
+      <c r="H27">
+        <v>1.53</v>
       </c>
       <c r="I27" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2091,28 +2079,28 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" t="s">
-        <v>10</v>
+        <v>131</v>
+      </c>
+      <c r="H28">
+        <v>0.42299999999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2120,144 +2108,28 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E29" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="F29" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="G29" t="s">
-        <v>122</v>
-      </c>
-      <c r="H29" t="s">
-        <v>124</v>
+        <v>137</v>
+      </c>
+      <c r="H29">
+        <v>1.32</v>
       </c>
       <c r="I29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" t="s">
-        <v>125</v>
-      </c>
-      <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30">
-        <v>2.72</v>
-      </c>
-      <c r="I30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31">
-        <v>1.53</v>
-      </c>
-      <c r="I31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2</v>
-      </c>
-      <c r="B32" t="s">
-        <v>137</v>
-      </c>
-      <c r="C32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D32" t="s">
         <v>136</v>
-      </c>
-      <c r="E32" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" t="s">
-        <v>134</v>
-      </c>
-      <c r="H32">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="I32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C33" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" t="s">
-        <v>138</v>
-      </c>
-      <c r="F33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33" t="s">
-        <v>140</v>
-      </c>
-      <c r="H33">
-        <v>1.32</v>
-      </c>
-      <c r="I33" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed BOM with categories and unit price
</commit_message>
<xml_diff>
--- a/Beaglebone CAN Cape BOM.xlsx
+++ b/Beaglebone CAN Cape BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="169">
   <si>
     <t>Qty</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Header, Female socket, .1"", 1-row, 6-pos</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>B130-13-F</t>
   </si>
   <si>
@@ -372,9 +369,6 @@
     <t>A106443-ND</t>
   </si>
   <si>
-    <t>Header, .1"", 2-row, 72-pos, breakable (Short Pins)</t>
-  </si>
-  <si>
     <t>BSS84</t>
   </si>
   <si>
@@ -387,9 +381,6 @@
     <t>P-Channel Enhancement Mode Field-Effect Transistor, -0.13 A, -50 V, SOT-23</t>
   </si>
   <si>
-    <t>REF197</t>
-  </si>
-  <si>
     <t>43045-0621</t>
   </si>
   <si>
@@ -529,6 +520,12 @@
   </si>
   <si>
     <t>X-518, X-519</t>
+  </si>
+  <si>
+    <t>Header, .1", 2-row, 72-pos, breakable (Short Pins)</t>
+  </si>
+  <si>
+    <t>Semiconductors</t>
   </si>
 </sst>
 </file>
@@ -1338,20 +1335,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="8" max="8" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1367,22 +1364,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1390,28 +1387,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H2" s="1">
-        <v>0.872</v>
+        <v>5.23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1419,28 +1416,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="H3" s="1">
-        <v>1.06</v>
+        <v>1.8</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1448,144 +1445,144 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>114</v>
+        <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.42</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>168</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>118</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.03</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>10</v>
+        <v>64</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="H7" s="1">
-        <v>0.82</v>
+        <v>0.03</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>135</v>
+        <v>73</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>136</v>
+        <v>75</v>
       </c>
       <c r="H8" s="1">
-        <v>0.91</v>
+        <v>0.2</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>169</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1593,144 +1590,144 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="H9" s="1">
-        <v>0.43</v>
+        <v>500</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
+      </c>
+      <c r="H10" s="1">
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>166</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="H11" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>0.872</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="H12" s="1">
-        <v>0.80300000000000005</v>
+        <v>0.82</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>134</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="H13" s="1">
-        <v>0.32</v>
+        <v>0.91</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1738,144 +1735,144 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="H14" s="1">
-        <v>1.2E-2</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>10</v>
+        <v>130</v>
+      </c>
+      <c r="H15" s="1">
+        <v>7.68</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="H16" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>2.72</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="H17" s="1">
-        <v>9.6000000000000002E-2</v>
+        <v>1.53</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>10</v>
+        <v>151</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.32</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1883,86 +1880,86 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="H19" s="1">
-        <v>7.68</v>
+        <v>0.43</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>131</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="H20" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>61</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>96</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="H21" s="1">
-        <v>9.0999999999999998E-2</v>
+        <v>0.32</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1970,86 +1967,86 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.2E-2</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H23" s="1">
-        <v>0.35499999999999998</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="H24" s="1">
-        <v>0.248</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2057,28 +2054,28 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>140</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1">
-        <v>2.72</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>139</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2086,28 +2083,28 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>146</v>
+        <v>72</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>140</v>
+        <v>38</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>145</v>
+        <v>71</v>
       </c>
       <c r="H26" s="1">
-        <v>1.53</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>144</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2115,28 +2112,28 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.248</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2144,28 +2141,28 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H28" s="1">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2173,28 +2170,28 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H29" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2202,28 +2199,28 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H30" s="1">
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2231,28 +2228,28 @@
         <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="H31" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2260,28 +2257,28 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H32" s="1">
         <v>0.47</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2289,28 +2286,28 @@
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H33" s="1">
         <v>0.42299999999999999</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2318,28 +2315,28 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>140</v>
+        <v>29</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>152</v>
+        <v>27</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>154</v>
+        <v>30</v>
       </c>
       <c r="H34" s="1">
-        <v>1.32</v>
+        <v>0.76200000000000001</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2347,33 +2344,33 @@
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>31</v>
+        <v>106</v>
       </c>
       <c r="H35" s="1">
-        <v>0.76200000000000001</v>
+        <v>1.06</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:I37">
-    <sortCondition ref="E2:E37"/>
+  <sortState ref="A2:I35">
+    <sortCondition ref="C2:C35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>